<commit_message>
test transactions multiparser - single sheet.
</commit_message>
<xml_diff>
--- a/test/fixtures/files/multi.xlsx
+++ b/test/fixtures/files/multi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiralles/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiralles/dev/stash/5411-IM-API/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30427CE0-5C80-2D46-AE91-F438992F3F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A612E3-C69C-8749-9E86-133D936DF41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" xr2:uid="{86C18E18-DAC6-784A-8A7F-C7EB184160F0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="407">
   <si>
     <t>XXS</t>
   </si>
@@ -1255,6 +1255,9 @@
   </si>
   <si>
     <t>COLOR</t>
+  </si>
+  <si>
+    <t>GREEN</t>
   </si>
 </sst>
 </file>
@@ -1769,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2EFE320-F95A-D44C-8F54-68A76C2EDE0A}">
   <dimension ref="A2:I285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1823,8 +1826,12 @@
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
       <c r="D4" s="3">
         <v>20</v>
       </c>
@@ -1855,7 +1862,9 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3">
         <v>22</v>
@@ -1887,7 +1896,9 @@
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
         <v>15</v>
@@ -1919,7 +1930,9 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3">
@@ -1949,7 +1962,9 @@
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3">
@@ -1979,7 +1994,9 @@
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3">
         <v>11</v>
@@ -2013,7 +2030,9 @@
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3">
@@ -2043,7 +2062,9 @@
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3">
@@ -2073,7 +2094,9 @@
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3">
         <v>10</v>
@@ -2105,7 +2128,9 @@
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -2131,7 +2156,9 @@
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3">
@@ -2173,7 +2200,9 @@
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3">
@@ -2205,7 +2234,9 @@
       <c r="A28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3">
@@ -2235,7 +2266,9 @@
       <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -2261,7 +2294,9 @@
       <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3">
         <v>2</v>
@@ -2291,7 +2326,9 @@
       <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C34" s="3">
         <v>1</v>
       </c>
@@ -2327,7 +2364,9 @@
       <c r="A36" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -2353,7 +2392,9 @@
       <c r="A38" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3">
@@ -2379,7 +2420,9 @@
       <c r="A40" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -2405,7 +2448,9 @@
       <c r="A42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3">
@@ -2433,7 +2478,9 @@
       <c r="A44" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -2459,7 +2506,9 @@
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="4"/>
+      <c r="B46" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -2485,7 +2534,9 @@
       <c r="A48" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="4"/>
+      <c r="B48" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>

</xml_diff>